<commit_message>
Backup to GitHub - 2021.08.06
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/MLM_V3.0_IndianLiverPatient_Iteration_1_Summary.xlsx
+++ b/01_Classification/03_Output/MLM_V3.0_IndianLiverPatient_Iteration_1_Summary.xlsx
@@ -80,19 +80,19 @@
     <t>STC</t>
   </si>
   <si>
-    <t>{'penalty': 'l2', 'solver': 'newton-cg', 'C': 805}</t>
-  </si>
-  <si>
-    <t>{'n_estimators': 400, 'max_features': 'sqrt', 'criterion': 'entropy', 'max_depth': 5, 'min_samples_split': 2}</t>
-  </si>
-  <si>
-    <t>{'n_estimators': 200, 'max_features': 'auto', 'criterion': 'gini', 'max_depth': 7, 'min_samples_split': 5}</t>
-  </si>
-  <si>
-    <t>{'C': 31, 'kernel': 'rbf', 'gamma': 0.0029629161062498708}</t>
-  </si>
-  <si>
-    <t>{'learning_rate': 0.08607787434020686, 'depth': 4, 'l2_leaf_reg': 5, 'iterations': 100}</t>
+    <t>{'penalty': 'l2', 'solver': 'liblinear', 'C': 353}</t>
+  </si>
+  <si>
+    <t>{'n_estimators': 50, 'max_features': 'auto', 'criterion': 'gini', 'max_depth': 4, 'min_samples_split': 2}</t>
+  </si>
+  <si>
+    <t>{'n_estimators': 600, 'max_features': 'auto', 'criterion': 'gini', 'max_depth': 7, 'min_samples_split': 5}</t>
+  </si>
+  <si>
+    <t>{'C': 21, 'kernel': 'rbf', 'gamma': 0.005686054187335557}</t>
+  </si>
+  <si>
+    <t>{'learning_rate': 0.09232246106244313, 'depth': 3, 'l2_leaf_reg': 2, 'iterations': 100}</t>
   </si>
   <si>
     <t>{}</t>
@@ -550,37 +550,37 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="C2">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="I2">
-        <v>0.67</v>
+        <v>0.54</v>
       </c>
       <c r="J2">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="L2">
-        <v>0.83</v>
+        <v>0.72</v>
       </c>
       <c r="M2" t="s">
         <v>21</v>
@@ -591,34 +591,34 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.86</v>
+        <v>0.83</v>
       </c>
       <c r="C3">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="I3">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="J3">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="K3">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="L3">
         <v>0.82</v>
@@ -632,37 +632,37 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="C4">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="D4">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
       <c r="I4">
-        <v>0.87</v>
+        <v>0.79</v>
       </c>
       <c r="J4">
-        <v>0.87</v>
+        <v>0.82</v>
       </c>
       <c r="K4">
         <v>0.67</v>
       </c>
       <c r="L4">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
@@ -676,34 +676,34 @@
         <v>0.7</v>
       </c>
       <c r="C5">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="I5">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="K5">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="L5">
-        <v>0.72</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="M5" t="s">
         <v>24</v>
@@ -714,37 +714,37 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="C6">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="D6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>0.93</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I6">
-        <v>0.87</v>
+        <v>0.71</v>
       </c>
       <c r="J6">
-        <v>0.9</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="K6">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="L6">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="M6" t="s">
         <v>25</v>
@@ -758,34 +758,34 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="I7">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="J7">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="K7">
-        <v>0.83</v>
+        <v>0.78</v>
       </c>
       <c r="L7">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="M7" t="s">
         <v>26</v>
@@ -796,37 +796,37 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
       <c r="C8">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H8">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="I8">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="J8">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="K8">
-        <v>0.67</v>
+        <v>0.89</v>
       </c>
       <c r="L8">
-        <v>0.73</v>
+        <v>0.82</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
@@ -837,37 +837,37 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="J9">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="K9">
         <v>0.33</v>
       </c>
       <c r="L9">
-        <v>0.67</v>
+        <v>0.58</v>
       </c>
       <c r="M9" t="s">
         <v>26</v>
@@ -908,16 +908,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.55</v>
+        <v>0.42</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="E2">
-        <v>0.71</v>
+        <v>0.57</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -926,16 +926,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="D3">
-        <v>0.67</v>
+        <v>0.54</v>
       </c>
       <c r="E3">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -944,16 +944,16 @@
         <v>39</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="D4">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="E4">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="F4">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -962,16 +962,16 @@
         <v>40</v>
       </c>
       <c r="C5">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="D5">
-        <v>0.83</v>
+        <v>0.72</v>
       </c>
       <c r="E5">
-        <v>0.75</v>
+        <v>0.63</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -980,16 +980,16 @@
         <v>41</v>
       </c>
       <c r="C6">
-        <v>0.87</v>
+        <v>0.79</v>
       </c>
       <c r="D6">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="E6">
-        <v>0.77</v>
+        <v>0.65</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1000,16 +1000,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.62</v>
+        <v>0.57</v>
       </c>
       <c r="D7">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="E7">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1018,16 +1018,16 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="D8">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="E8">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1036,16 +1036,16 @@
         <v>39</v>
       </c>
       <c r="C9">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="D9">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E9">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="F9">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1054,16 +1054,16 @@
         <v>40</v>
       </c>
       <c r="C10">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="D10">
         <v>0.82</v>
       </c>
       <c r="E10">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1075,13 +1075,13 @@
         <v>0.84</v>
       </c>
       <c r="D11">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E11">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1092,16 +1092,16 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.62</v>
+        <v>0.57</v>
       </c>
       <c r="D12">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="E12">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1110,16 +1110,16 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="D13">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="E13">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="F13">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1128,16 +1128,16 @@
         <v>39</v>
       </c>
       <c r="C14">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="D14">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E14">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="F14">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1146,16 +1146,16 @@
         <v>40</v>
       </c>
       <c r="C15">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="D15">
         <v>0.82</v>
       </c>
       <c r="E15">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="F15">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1167,13 +1167,13 @@
         <v>0.84</v>
       </c>
       <c r="D16">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E16">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="F16">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1184,16 +1184,16 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D17">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="E17">
-        <v>0.59</v>
+        <v>0.55</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1202,16 +1202,16 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="D18">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E18">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1220,16 +1220,16 @@
         <v>39</v>
       </c>
       <c r="C19">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="D19">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="E19">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="F19">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C20">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="D20">
-        <v>0.72</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E20">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="F20">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1256,16 +1256,16 @@
         <v>41</v>
       </c>
       <c r="C21">
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="D21">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="E21">
-        <v>0.68</v>
+        <v>0.62</v>
       </c>
       <c r="F21">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1276,16 +1276,16 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="D22">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="E22">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1294,16 +1294,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0.93</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D23">
-        <v>0.87</v>
+        <v>0.71</v>
       </c>
       <c r="E23">
-        <v>0.9</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F23">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1312,16 +1312,16 @@
         <v>39</v>
       </c>
       <c r="C24">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="D24">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E24">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="F24">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1330,16 +1330,16 @@
         <v>40</v>
       </c>
       <c r="C25">
-        <v>0.82</v>
+        <v>0.74</v>
       </c>
       <c r="D25">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="E25">
-        <v>0.83</v>
+        <v>0.74</v>
       </c>
       <c r="F25">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1348,16 +1348,16 @@
         <v>41</v>
       </c>
       <c r="C26">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="D26">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E26">
-        <v>0.86</v>
+        <v>0.77</v>
       </c>
       <c r="F26">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1368,16 +1368,16 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>0.62</v>
+        <v>0.54</v>
       </c>
       <c r="D27">
-        <v>0.83</v>
+        <v>0.78</v>
       </c>
       <c r="E27">
-        <v>0.71</v>
+        <v>0.64</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1386,16 +1386,16 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="D28">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="E28">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="F28">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1404,16 +1404,16 @@
         <v>39</v>
       </c>
       <c r="C29">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="D29">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="E29">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="F29">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1422,16 +1422,16 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
       <c r="D30">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="E30">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="F30">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1440,16 +1440,16 @@
         <v>41</v>
       </c>
       <c r="C31">
-        <v>0.84</v>
+        <v>0.8</v>
       </c>
       <c r="D31">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="E31">
-        <v>0.82</v>
+        <v>0.77</v>
       </c>
       <c r="F31">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1463,13 +1463,13 @@
         <v>0.57</v>
       </c>
       <c r="D32">
-        <v>0.67</v>
+        <v>0.89</v>
       </c>
       <c r="E32">
-        <v>0.62</v>
+        <v>0.7</v>
       </c>
       <c r="F32">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1478,16 +1478,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="D33">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="E33">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="F33">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1496,16 +1496,16 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="D34">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="E34">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="F34">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1514,16 +1514,16 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>0.71</v>
+        <v>0.76</v>
       </c>
       <c r="D35">
-        <v>0.73</v>
+        <v>0.82</v>
       </c>
       <c r="E35">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="F35">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1532,16 +1532,16 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>0.78</v>
+        <v>0.84</v>
       </c>
       <c r="D36">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="E36">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="F36">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1552,16 +1552,16 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0.43</v>
       </c>
       <c r="D37">
         <v>0.33</v>
       </c>
       <c r="E37">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="F37">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1570,16 +1570,16 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="E38">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="F38">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1588,16 +1588,16 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="D39">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E39">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="F39">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1606,16 +1606,16 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>0.89</v>
+        <v>0.6</v>
       </c>
       <c r="D40">
-        <v>0.67</v>
+        <v>0.58</v>
       </c>
       <c r="E40">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="F40">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1624,16 +1624,16 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>0.85</v>
+        <v>0.68</v>
       </c>
       <c r="D41">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E41">
-        <v>0.77</v>
+        <v>0.68</v>
       </c>
       <c r="F41">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>